<commit_message>
modify table and script
</commit_message>
<xml_diff>
--- a/xlsx/s_TreasureInfo.xlsx
+++ b/xlsx/s_TreasureInfo.xlsx
@@ -55,7 +55,9 @@
         <sz val="10.0"/>
         <color rgb="FF000000"/>
       </rPr>
-      <t xml:space="preserve">[{"itemId":1, "rate":10, amount:1},{"itemId":2, "rate":30, amount:1},{"itemId":3, "rate":60, amount:1}]</t>
+      <t xml:space="preserve">itemid 对应item表中物品
+rate 出现概率
+amount 对应数量</t>
     </r>
     <phoneticPr fontId="1" type="noConversion" alignment="left"/>
   </si>
@@ -66,9 +68,7 @@
         <sz val="10.0"/>
         <color rgb="FF000000"/>
       </rPr>
-      <t xml:space="preserve">itemid 对应item表中物品
-rate 出现概率
-amount 对应数量</t>
+      <t xml:space="preserve">[{"itemId":1, "rate":10, amount:1},{"itemId":2, "rate":30, amount:1},{"itemId":3, "rate":60, amount:1}]</t>
     </r>
     <phoneticPr fontId="1" type="noConversion" alignment="left"/>
   </si>
@@ -323,7 +323,7 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:w="http://schemas.openxmlformats.org/wordprocessingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:w14="http://schemas.microsoft.com/office/word/2010/wordml" xmlns:wp="http://schemas.openxmlformats.org/drawingml/2006/wordprocessingDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:wp14="http://schemas.microsoft.com/office/word/2010/wordprocessingDrawing" xmlns:w15="http://schemas.microsoft.com/office/word/2012/wordml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:ns10="http://schemas.openxmlformats.org/schemaLibrary/2006/main" xmlns:wne="http://schemas.microsoft.com/office/word/2006/wordml" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:ns13="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:ns20="urn:schemas-microsoft-com:office:excel" xmlns:w10="urn:schemas-microsoft-com:office:word" xmlns:ns22="urn:schemas-microsoft-com:office:powerpoint" xmlns:ns24="http://schemas.microsoft.com/office/2006/coverPageProps" xmlns:odx="http://opendope.org/xpaths" xmlns:odc="http://opendope.org/conditions" xmlns:odq="http://opendope.org/questions" xmlns:oda="http://opendope.org/answers" xmlns:odi="http://opendope.org/components" xmlns:odgm="http://opendope.org/SmartArt/DataHierarchy" xmlns:b="http://schemas.openxmlformats.org/officeDocument/2006/bibliography" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11" xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" xmlns:ns34="http://schemas.openxmlformats.org/drawingml/2006/compatibility" xmlns:ns35="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas">
+<xdr:wsDr xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:w="http://schemas.openxmlformats.org/wordprocessingml/2006/main" xmlns:w15="http://schemas.microsoft.com/office/word/2012/wordml" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:w14="http://schemas.microsoft.com/office/word/2010/wordml" xmlns:wp="http://schemas.openxmlformats.org/drawingml/2006/wordprocessingDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:wp14="http://schemas.microsoft.com/office/word/2010/wordprocessingDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:ns10="http://schemas.openxmlformats.org/schemaLibrary/2006/main" xmlns:wne="http://schemas.microsoft.com/office/word/2006/wordml" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:ns13="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:ns20="urn:schemas-microsoft-com:office:excel" xmlns:w10="urn:schemas-microsoft-com:office:word" xmlns:ns22="urn:schemas-microsoft-com:office:powerpoint" xmlns:ns24="http://schemas.microsoft.com/office/2006/coverPageProps" xmlns:odx="http://opendope.org/xpaths" xmlns:odc="http://opendope.org/conditions" xmlns:odq="http://opendope.org/questions" xmlns:oda="http://opendope.org/answers" xmlns:odi="http://opendope.org/components" xmlns:odgm="http://opendope.org/SmartArt/DataHierarchy" xmlns:b="http://schemas.openxmlformats.org/officeDocument/2006/bibliography" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11" xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" xmlns:ns34="http://schemas.openxmlformats.org/drawingml/2006/compatibility" xmlns:ns35="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
@@ -372,7 +372,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:w="http://schemas.openxmlformats.org/wordprocessingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:w14="http://schemas.microsoft.com/office/word/2010/wordml" xmlns:wp="http://schemas.openxmlformats.org/drawingml/2006/wordprocessingDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:wp14="http://schemas.microsoft.com/office/word/2010/wordprocessingDrawing" xmlns:w15="http://schemas.microsoft.com/office/word/2012/wordml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:ns10="http://schemas.openxmlformats.org/schemaLibrary/2006/main" xmlns:wne="http://schemas.microsoft.com/office/word/2006/wordml" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:ns13="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:ns20="urn:schemas-microsoft-com:office:excel" xmlns:w10="urn:schemas-microsoft-com:office:word" xmlns:ns22="urn:schemas-microsoft-com:office:powerpoint" xmlns:ns24="http://schemas.microsoft.com/office/2006/coverPageProps" xmlns:odx="http://opendope.org/xpaths" xmlns:odc="http://opendope.org/conditions" xmlns:odq="http://opendope.org/questions" xmlns:oda="http://opendope.org/answers" xmlns:odi="http://opendope.org/components" xmlns:odgm="http://opendope.org/SmartArt/DataHierarchy" xmlns:b="http://schemas.openxmlformats.org/officeDocument/2006/bibliography" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11" xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" xmlns:ns34="http://schemas.openxmlformats.org/drawingml/2006/compatibility" xmlns:ns35="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas" name="Office 主题">
+<a:theme xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:w="http://schemas.openxmlformats.org/wordprocessingml/2006/main" xmlns:w15="http://schemas.microsoft.com/office/word/2012/wordml" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:w14="http://schemas.microsoft.com/office/word/2010/wordml" xmlns:wp="http://schemas.openxmlformats.org/drawingml/2006/wordprocessingDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:wp14="http://schemas.microsoft.com/office/word/2010/wordprocessingDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:ns10="http://schemas.openxmlformats.org/schemaLibrary/2006/main" xmlns:wne="http://schemas.microsoft.com/office/word/2006/wordml" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:ns13="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:ns20="urn:schemas-microsoft-com:office:excel" xmlns:w10="urn:schemas-microsoft-com:office:word" xmlns:ns22="urn:schemas-microsoft-com:office:powerpoint" xmlns:ns24="http://schemas.microsoft.com/office/2006/coverPageProps" xmlns:odx="http://opendope.org/xpaths" xmlns:odc="http://opendope.org/conditions" xmlns:odq="http://opendope.org/questions" xmlns:oda="http://opendope.org/answers" xmlns:odi="http://opendope.org/components" xmlns:odgm="http://opendope.org/SmartArt/DataHierarchy" xmlns:b="http://schemas.openxmlformats.org/officeDocument/2006/bibliography" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11" xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" xmlns:ns34="http://schemas.openxmlformats.org/drawingml/2006/compatibility" xmlns:ns35="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -663,10 +663,10 @@
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="15.6" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="6.746987951807228" customWidth="true"/>
-    <col min="2" max="2" width="77.95180722891565" customWidth="true"/>
-    <col min="3" max="3" width="32.53012048192771" customWidth="true"/>
-    <col min="4" max="4" width="12.89156626506024" customWidth="true"/>
-    <col min="5" max="5" width="43.373493975903614" customWidth="true"/>
+    <col min="2" max="2" width="32.53012048192771" customWidth="true"/>
+    <col min="3" max="3" width="77.95180722891565" customWidth="true"/>
+    <col min="4" max="4" width="43.373493975903614" customWidth="true"/>
+    <col min="5" max="5" width="12.89156626506024" customWidth="true"/>
     <col min="6" max="6" width="12.89156626506024" customWidth="true"/>
     <col min="7" max="7" width="12.89156626506024" customWidth="true"/>
     <col min="8" max="8" width="12.89156626506024" customWidth="true"/>
@@ -694,14 +694,14 @@
       <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="24"/>
+      <c r="C1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="24"/>
+      <c r="E1" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="24"/>
       <c r="F1" s="24"/>
       <c r="G1" s="24"/>
       <c r="H1" s="24"/>
@@ -728,17 +728,17 @@
       <c r="A2" s="25" t="n">
         <v>1.0</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="25" t="n">
+      <c r="D2" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="25" t="n">
         <v>1.0</v>
-      </c>
-      <c r="E2" s="26" t="s">
-        <v>5</v>
       </c>
       <c r="F2" s="24"/>
       <c r="G2" s="24"/>
@@ -766,14 +766,14 @@
       <c r="A3" s="25" t="n">
         <v>2.0</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="24"/>
+      <c r="C3" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="24"/>
-      <c r="D3" s="25" t="n">
+      <c r="D3" s="24"/>
+      <c r="E3" s="25" t="n">
         <v>1.0</v>
       </c>
-      <c r="E3" s="24"/>
       <c r="F3" s="24"/>
       <c r="G3" s="24"/>
       <c r="H3" s="24"/>

</xml_diff>